<commit_message>
Subo cambios en Gestion documental (cambio de fecha, cotizacion de todos los tipos de poliza, emision de prendario, cambio de fecha y refacturacion)
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Endoso Inclusion de Riesgo - Vehiculos.xlsx
+++ b/Sura/DataSource - Endoso Inclusion de Riesgo - Vehiculos.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CED188-CA95-4095-BE13-E754C0266275}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB44651-455A-4575-83F1-036B0243AE51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0178C8D5-B58C-4945-A4FB-75B1608B42A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Anio</t>
   </si>
@@ -66,10 +63,19 @@
     <t>Sin Actividad</t>
   </si>
   <si>
-    <t>ONIX 1.2 L/20</t>
-  </si>
-  <si>
-    <t>ONIX 1.2 L/21</t>
+    <t>ONIX 1.2 L/25</t>
+  </si>
+  <si>
+    <t>ZZZ111BB00</t>
+  </si>
+  <si>
+    <t>ZZZ111BB0011</t>
+  </si>
+  <si>
+    <t>ZZZ112</t>
+  </si>
+  <si>
+    <t>ZZZ113</t>
   </si>
 </sst>
 </file>
@@ -128,53 +134,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Emisión_Motor"/>
-      <sheetName val="Motor_Answer"/>
-      <sheetName val="EmisionFlota"/>
-      <sheetName val="EmisionAP"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>i-preproducciongestion.segurossura.com.ar</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="R4" t="str">
-            <v>AON003</v>
-          </cell>
-          <cell r="S4" t="str">
-            <v>ABC12AON003</v>
-          </cell>
-          <cell r="T4" t="str">
-            <v>ZAZ12AON003</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="R5" t="str">
-            <v>AON004</v>
-          </cell>
-          <cell r="S5" t="str">
-            <v>ABC12AON004</v>
-          </cell>
-          <cell r="T5" t="str">
-            <v>ZAZ12AON004</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -477,7 +436,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,17 +497,14 @@
       <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="str">
-        <f>[1]Emisión_Motor!$R4</f>
-        <v>AON003</v>
-      </c>
-      <c r="G2" t="str">
-        <f>[1]Emisión_Motor!$S4</f>
-        <v>ABC12AON003</v>
-      </c>
-      <c r="H2" t="str">
-        <f>[1]Emisión_Motor!$T4</f>
-        <v>ZAZ12AON003</v>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
       </c>
       <c r="I2" t="s">
         <v>11</v>
@@ -562,25 +518,22 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3">
-        <v>1700000</v>
+        <v>1700001</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="str">
-        <f>[1]Emisión_Motor!$R5</f>
-        <v>AON004</v>
-      </c>
-      <c r="G3" t="str">
-        <f>[1]Emisión_Motor!$S5</f>
-        <v>ABC12AON004</v>
-      </c>
-      <c r="H3" t="str">
-        <f>[1]Emisión_Motor!$T5</f>
-        <v>ZAZ12AON004</v>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>

</xml_diff>